<commit_message>
changed data sets names
</commit_message>
<xml_diff>
--- a/Data/Processed/Rainfall.xlsx
+++ b/Data/Processed/Rainfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\pet-inflation\Data\Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0D9485-0D59-48D5-AF81-633983A18C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FCB793-A087-45F0-B9D0-A9109D36276B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6950,7 +6950,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4395D6D4-7129-4C21-8B13-39E857F6DFD7}" name="rainfall_UK" displayName="rainfall_UK" ref="A1:B2281" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B2281" xr:uid="{4395D6D4-7129-4C21-8B13-39E857F6DFD7}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{31BFC12F-4B3F-4BAB-81D0-8A05DAB5819D}" uniqueName="1" name="Date" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{A1E171DD-7DD8-41D7-BF9C-29C81F25C1C9}" uniqueName="2" name="Value" queryTableFieldId="2"/>
@@ -7225,7 +7224,7 @@
   <dimension ref="A1:B2281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>